<commit_message>
Minor changes assoicated with adding folders on GitHub repo
</commit_message>
<xml_diff>
--- a/Climate station data.xlsx
+++ b/Climate station data.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11002"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11006"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{FD478936-077F-D04B-809A-3D2F92A7F637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF351ADD-F310-704A-8546-A05934AF9C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="1480" windowWidth="27240" windowHeight="15940"/>
+    <workbookView xWindow="1560" yWindow="1480" windowWidth="27240" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Climate station data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -142,7 +152,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -976,11 +986,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1088,8 +1098,8 @@
         <v>1</v>
       </c>
       <c r="Q2">
-        <f>N2-K2</f>
-        <v>80</v>
+        <f>N2-K2+1</f>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -1142,8 +1152,8 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <f>N3-K3</f>
-        <v>80</v>
+        <f>N3-K3+1</f>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -1196,8 +1206,8 @@
         <v>1</v>
       </c>
       <c r="Q4">
-        <f>N4-K4</f>
-        <v>23</v>
+        <f>N4-K4+1</f>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added climate data files that Rachael downloaded
</commit_message>
<xml_diff>
--- a/Climate station data.xlsx
+++ b/Climate station data.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11006"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\racha\Desktop\insect_responses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF351ADD-F310-704A-8546-A05934AF9C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432CD1B8-A95F-46A7-B2C8-D06CB506ED69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1480" windowWidth="27240" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Climate station data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
   <si>
     <t>Species</t>
   </si>
@@ -147,13 +146,61 @@
   </si>
   <si>
     <t>End_day</t>
+  </si>
+  <si>
+    <t>OUAGADOUGOU</t>
+  </si>
+  <si>
+    <t>UVM00065503</t>
+  </si>
+  <si>
+    <t>DONGTAI</t>
+  </si>
+  <si>
+    <t>CHM00058251</t>
+  </si>
+  <si>
+    <t>CHM00058252</t>
+  </si>
+  <si>
+    <t>BEIJING</t>
+  </si>
+  <si>
+    <t>CHM00054511</t>
+  </si>
+  <si>
+    <t>ANYANG</t>
+  </si>
+  <si>
+    <t>CHM00053898</t>
+  </si>
+  <si>
+    <t>HELLINIKON</t>
+  </si>
+  <si>
+    <t>GR000016716</t>
+  </si>
+  <si>
+    <t>GR000016717</t>
+  </si>
+  <si>
+    <t>JUIZ_DE_FORA</t>
+  </si>
+  <si>
+    <t>BR002143012</t>
+  </si>
+  <si>
+    <t>BR002143013</t>
+  </si>
+  <si>
+    <t>BR002143014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -284,6 +331,19 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -630,8 +690,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -989,13 +1052,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12:Q14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1048,7 +1111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1102,7 +1165,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1152,11 +1215,11 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <f>N3-K3+1</f>
+        <f t="shared" ref="Q3:Q14" si="0">N3-K3+1</f>
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1206,11 +1269,11 @@
         <v>1</v>
       </c>
       <c r="Q4">
-        <f>N4-K4+1</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1223,8 +1286,48 @@
       <c r="D5" t="s">
         <v>13</v>
       </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5">
+        <v>12.35</v>
+      </c>
+      <c r="G5">
+        <v>-1.51</v>
+      </c>
+      <c r="H5">
+        <v>316</v>
+      </c>
+      <c r="I5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5">
+        <v>65503</v>
+      </c>
+      <c r="K5">
+        <v>1973</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>2021</v>
+      </c>
+      <c r="O5">
+        <v>10</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1237,8 +1340,48 @@
       <c r="D6" t="s">
         <v>13</v>
       </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6">
+        <v>32.85</v>
+      </c>
+      <c r="G6">
+        <v>120.28</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="1">
+        <v>58251</v>
+      </c>
+      <c r="K6">
+        <v>1953</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>2021</v>
+      </c>
+      <c r="O6">
+        <v>10</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1251,8 +1394,48 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7">
+        <v>32.85</v>
+      </c>
+      <c r="G7">
+        <v>120.28</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="1">
+        <v>58251</v>
+      </c>
+      <c r="K7">
+        <v>1953</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>2021</v>
+      </c>
+      <c r="O7">
+        <v>10</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1265,8 +1448,48 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8">
+        <v>39.93</v>
+      </c>
+      <c r="G8">
+        <v>116.28</v>
+      </c>
+      <c r="H8">
+        <v>55</v>
+      </c>
+      <c r="I8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8">
+        <v>54511</v>
+      </c>
+      <c r="K8">
+        <v>1951</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>2021</v>
+      </c>
+      <c r="O8">
+        <v>9</v>
+      </c>
+      <c r="P8">
+        <v>29</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1279,8 +1502,48 @@
       <c r="D9" t="s">
         <v>13</v>
       </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9">
+        <v>36.049999999999997</v>
+      </c>
+      <c r="G9">
+        <v>114.4</v>
+      </c>
+      <c r="H9">
+        <v>64</v>
+      </c>
+      <c r="I9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9">
+        <v>53898</v>
+      </c>
+      <c r="K9">
+        <v>1951</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>2021</v>
+      </c>
+      <c r="O9">
+        <v>10</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1293,8 +1556,48 @@
       <c r="D10" t="s">
         <v>13</v>
       </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10">
+        <v>37.9</v>
+      </c>
+      <c r="G10">
+        <v>23.75</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10">
+        <v>16716</v>
+      </c>
+      <c r="K10">
+        <v>1955</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>2021</v>
+      </c>
+      <c r="O10">
+        <v>10</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1307,13 +1610,53 @@
       <c r="D11" t="s">
         <v>13</v>
       </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11">
+        <v>37.9</v>
+      </c>
+      <c r="G11">
+        <v>23.75</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11">
+        <v>16716</v>
+      </c>
+      <c r="K11">
+        <v>1955</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>2021</v>
+      </c>
+      <c r="O11">
+        <v>10</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
       <c r="B12">
-        <v>21.23</v>
+        <v>-21.23</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1321,13 +1664,53 @@
       <c r="D12" t="s">
         <v>30</v>
       </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12">
+        <v>-21.77</v>
+      </c>
+      <c r="G12">
+        <v>-43.35</v>
+      </c>
+      <c r="H12">
+        <v>911</v>
+      </c>
+      <c r="I12" t="s">
+        <v>52</v>
+      </c>
+      <c r="J12">
+        <v>83692</v>
+      </c>
+      <c r="K12">
+        <v>1977</v>
+      </c>
+      <c r="L12">
+        <v>10</v>
+      </c>
+      <c r="M12">
+        <v>24</v>
+      </c>
+      <c r="N12">
+        <v>2017</v>
+      </c>
+      <c r="O12">
+        <v>8</v>
+      </c>
+      <c r="P12">
+        <v>7</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>31</v>
       </c>
       <c r="B13">
-        <v>21.23</v>
+        <v>-21.23</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -1335,13 +1718,50 @@
       <c r="D13" t="s">
         <v>30</v>
       </c>
+      <c r="F13">
+        <v>-21.77</v>
+      </c>
+      <c r="G13">
+        <v>-43.35</v>
+      </c>
+      <c r="H13">
+        <v>911</v>
+      </c>
+      <c r="I13" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13">
+        <v>83692</v>
+      </c>
+      <c r="K13">
+        <v>1977</v>
+      </c>
+      <c r="L13">
+        <v>10</v>
+      </c>
+      <c r="M13">
+        <v>24</v>
+      </c>
+      <c r="N13">
+        <v>2017</v>
+      </c>
+      <c r="O13">
+        <v>8</v>
+      </c>
+      <c r="P13">
+        <v>7</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
       <c r="B14">
-        <v>21.23</v>
+        <v>-21.23</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -1349,8 +1769,47 @@
       <c r="D14" t="s">
         <v>30</v>
       </c>
+      <c r="F14">
+        <v>-21.77</v>
+      </c>
+      <c r="G14">
+        <v>-43.35</v>
+      </c>
+      <c r="H14">
+        <v>911</v>
+      </c>
+      <c r="I14" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14">
+        <v>83692</v>
+      </c>
+      <c r="K14">
+        <v>1977</v>
+      </c>
+      <c r="L14">
+        <v>10</v>
+      </c>
+      <c r="M14">
+        <v>24</v>
+      </c>
+      <c r="N14">
+        <v>2017</v>
+      </c>
+      <c r="O14">
+        <v>8</v>
+      </c>
+      <c r="P14">
+        <v>7</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed problem with temperature function and re-did TPC and model analyses
</commit_message>
<xml_diff>
--- a/Climate station data.xlsx
+++ b/Climate station data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\racha\Desktop\insect_responses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432CD1B8-A95F-46A7-B2C8-D06CB506ED69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048DD0C2-B081-4F86-9CD1-9F205D05D3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="117">
   <si>
     <t>Species</t>
   </si>
@@ -194,6 +194,192 @@
   </si>
   <si>
     <t>BR002143014</t>
+  </si>
+  <si>
+    <t>Subtropical</t>
+  </si>
+  <si>
+    <t>JA000047682</t>
+  </si>
+  <si>
+    <t>LEEMING</t>
+  </si>
+  <si>
+    <t>UKM00003257</t>
+  </si>
+  <si>
+    <t>CHIBA</t>
+  </si>
+  <si>
+    <t>JA000047683</t>
+  </si>
+  <si>
+    <t>JA000047684</t>
+  </si>
+  <si>
+    <t>KOCHI</t>
+  </si>
+  <si>
+    <t>JA000047893</t>
+  </si>
+  <si>
+    <t>HOMESTEAD_GEN_AVIATION_AP,_FL</t>
+  </si>
+  <si>
+    <t>USC00084095</t>
+  </si>
+  <si>
+    <t>Pilophorus typicus Japan Kochi</t>
+  </si>
+  <si>
+    <t>Toxoptera citricidus Japan Chiba</t>
+  </si>
+  <si>
+    <t>Aphis citricola Japan Chiba</t>
+  </si>
+  <si>
+    <t>Aphis gossypii Japan Chiba</t>
+  </si>
+  <si>
+    <t>Acyrthosiphon pisum UK Sand Hutton</t>
+  </si>
+  <si>
+    <t>Bemisia argentifollii US Homestead</t>
+  </si>
+  <si>
+    <t>Rhopalosiphum rufiabdominalis US Naples</t>
+  </si>
+  <si>
+    <t>NAPLES,_FL</t>
+  </si>
+  <si>
+    <t>USC00086078</t>
+  </si>
+  <si>
+    <t>Aphis nasturtii US Weston</t>
+  </si>
+  <si>
+    <t>FT_LAUDERDALE,_FL</t>
+  </si>
+  <si>
+    <t>USC00083163</t>
+  </si>
+  <si>
+    <t>Diaphorina citri US Pompano Beach</t>
+  </si>
+  <si>
+    <t>POMPANO_BEACH_AIRPARK,_FL</t>
+  </si>
+  <si>
+    <t>USW00092805</t>
+  </si>
+  <si>
+    <t>LUBBOCK,_TX</t>
+  </si>
+  <si>
+    <t>USW00023042</t>
+  </si>
+  <si>
+    <t>Aphis gossypii USA Lubbock</t>
+  </si>
+  <si>
+    <t>Drepanosiphum platanoidis UK Norwich</t>
+  </si>
+  <si>
+    <t>Drepanosiphum acerinum UK Norwich</t>
+  </si>
+  <si>
+    <t>Macrosiphum euphorbiae Canada</t>
+  </si>
+  <si>
+    <t>Myzus persicae Canada</t>
+  </si>
+  <si>
+    <t>SARNIA_CLIMATE,_ON</t>
+  </si>
+  <si>
+    <t>CA006127519</t>
+  </si>
+  <si>
+    <t>Eriosoma lanigerum Australia Yathroo</t>
+  </si>
+  <si>
+    <t>WONGAN_HILLS</t>
+  </si>
+  <si>
+    <t>ASN00008137</t>
+  </si>
+  <si>
+    <t>CA006127520</t>
+  </si>
+  <si>
+    <t>Hyperomyzus lactucae Australia Acton</t>
+  </si>
+  <si>
+    <t>CANBERRA_AIRPORT_COMPARISON</t>
+  </si>
+  <si>
+    <t>ASN00070014</t>
+  </si>
+  <si>
+    <t>Aphis gossypii Iran</t>
+  </si>
+  <si>
+    <t>Aphis gossypii China Henan</t>
+  </si>
+  <si>
+    <t>Aulacorthum solani US Ithaca</t>
+  </si>
+  <si>
+    <t>ITHACA_CORNELL_UNIV,_NY</t>
+  </si>
+  <si>
+    <t>USC00304174</t>
+  </si>
+  <si>
+    <t>Brevicoryne brassicae US Columbia</t>
+  </si>
+  <si>
+    <t>COLUMBIA_U_OF_M,_MO</t>
+  </si>
+  <si>
+    <t>USC00231801</t>
+  </si>
+  <si>
+    <t>Myzus persicae US Columbia</t>
+  </si>
+  <si>
+    <t>Hyadaphis pseudobrassicae US Columbia</t>
+  </si>
+  <si>
+    <t>USC00231802</t>
+  </si>
+  <si>
+    <t>USC00231803</t>
+  </si>
+  <si>
+    <t>Lygus lineolaris US Leland</t>
+  </si>
+  <si>
+    <t>STONEVILLE_EXP_STN,_MS</t>
+  </si>
+  <si>
+    <t>USC00228445</t>
+  </si>
+  <si>
+    <t>LOWESTOFT</t>
+  </si>
+  <si>
+    <t>UKE00105899</t>
+  </si>
+  <si>
+    <t>UKE00105900</t>
+  </si>
+  <si>
+    <t>TEHRAN-MEHRABAD</t>
+  </si>
+  <si>
+    <t>IR000407540</t>
   </si>
 </sst>
 </file>
@@ -690,11 +876,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1050,13 +1237,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12:Q14"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.08203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1215,7 +1405,7 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q14" si="0">N3-K3+1</f>
+        <f t="shared" ref="Q3:Q37" si="0">N3-K3+1</f>
         <v>81</v>
       </c>
     </row>
@@ -1718,6 +1908,9 @@
       <c r="D13" t="s">
         <v>30</v>
       </c>
+      <c r="E13" t="s">
+        <v>51</v>
+      </c>
       <c r="F13">
         <v>-21.77</v>
       </c>
@@ -1769,6 +1962,9 @@
       <c r="D14" t="s">
         <v>30</v>
       </c>
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
       <c r="F14">
         <v>-21.77</v>
       </c>
@@ -1805,6 +2001,1212 @@
       <c r="Q14">
         <f t="shared" si="0"/>
         <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15">
+        <v>33.619999999999997</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15">
+        <v>33.57</v>
+      </c>
+      <c r="G15">
+        <v>133.35</v>
+      </c>
+      <c r="H15">
+        <v>5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15">
+        <v>47893</v>
+      </c>
+      <c r="K15">
+        <v>1951</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>2021</v>
+      </c>
+      <c r="O15">
+        <v>9</v>
+      </c>
+      <c r="P15">
+        <v>30</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16">
+        <v>33.42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16">
+        <v>33.43</v>
+      </c>
+      <c r="G16">
+        <v>-90.9</v>
+      </c>
+      <c r="H16">
+        <v>39</v>
+      </c>
+      <c r="I16" t="s">
+        <v>111</v>
+      </c>
+      <c r="K16">
+        <v>1930</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>2019</v>
+      </c>
+      <c r="O16">
+        <v>4</v>
+      </c>
+      <c r="P16">
+        <v>30</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17">
+        <v>35.380000000000003</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17">
+        <v>35.6</v>
+      </c>
+      <c r="G17">
+        <v>140.1</v>
+      </c>
+      <c r="H17">
+        <v>19</v>
+      </c>
+      <c r="I17" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17">
+        <v>47682</v>
+      </c>
+      <c r="K17">
+        <v>1967</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>2021</v>
+      </c>
+      <c r="O17">
+        <v>10</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18">
+        <v>35.380000000000003</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18">
+        <v>35.6</v>
+      </c>
+      <c r="G18">
+        <v>140.1</v>
+      </c>
+      <c r="H18">
+        <v>19</v>
+      </c>
+      <c r="I18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18">
+        <v>47682</v>
+      </c>
+      <c r="K18">
+        <v>1967</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>2021</v>
+      </c>
+      <c r="O18">
+        <v>10</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19">
+        <v>35.380000000000003</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19">
+        <v>35.6</v>
+      </c>
+      <c r="G19">
+        <v>140.1</v>
+      </c>
+      <c r="H19">
+        <v>19</v>
+      </c>
+      <c r="I19" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19">
+        <v>47682</v>
+      </c>
+      <c r="K19">
+        <v>1967</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>2021</v>
+      </c>
+      <c r="O19">
+        <v>10</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20">
+        <v>54.02</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20">
+        <v>54.3</v>
+      </c>
+      <c r="G20">
+        <v>-1.53</v>
+      </c>
+      <c r="H20">
+        <v>40</v>
+      </c>
+      <c r="I20" t="s">
+        <v>58</v>
+      </c>
+      <c r="J20">
+        <v>3257</v>
+      </c>
+      <c r="K20">
+        <v>1973</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>2021</v>
+      </c>
+      <c r="O20">
+        <v>10</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21">
+        <v>25.47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21">
+        <v>25.5</v>
+      </c>
+      <c r="G21">
+        <v>-80.55</v>
+      </c>
+      <c r="H21">
+        <v>3</v>
+      </c>
+      <c r="I21" t="s">
+        <v>65</v>
+      </c>
+      <c r="K21">
+        <v>1990</v>
+      </c>
+      <c r="L21">
+        <v>6</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>2021</v>
+      </c>
+      <c r="O21">
+        <v>10</v>
+      </c>
+      <c r="P21">
+        <v>2</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22">
+        <v>26.14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22">
+        <v>26.17</v>
+      </c>
+      <c r="G22">
+        <v>-81.680000000000007</v>
+      </c>
+      <c r="H22">
+        <v>12</v>
+      </c>
+      <c r="I22" t="s">
+        <v>74</v>
+      </c>
+      <c r="K22">
+        <v>1942</v>
+      </c>
+      <c r="L22">
+        <v>3</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>2021</v>
+      </c>
+      <c r="O22">
+        <v>10</v>
+      </c>
+      <c r="P22">
+        <v>2</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23">
+        <v>26.14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23">
+        <v>26.1</v>
+      </c>
+      <c r="G23">
+        <v>-80.2</v>
+      </c>
+      <c r="H23">
+        <v>5</v>
+      </c>
+      <c r="I23" t="s">
+        <v>77</v>
+      </c>
+      <c r="K23">
+        <v>1912</v>
+      </c>
+      <c r="L23">
+        <v>11</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>2021</v>
+      </c>
+      <c r="O23">
+        <v>10</v>
+      </c>
+      <c r="P23">
+        <v>2</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24">
+        <v>26.24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24">
+        <v>26.25</v>
+      </c>
+      <c r="G24">
+        <v>-80.11</v>
+      </c>
+      <c r="H24">
+        <v>6</v>
+      </c>
+      <c r="I24" t="s">
+        <v>80</v>
+      </c>
+      <c r="K24">
+        <v>1998</v>
+      </c>
+      <c r="L24">
+        <v>3</v>
+      </c>
+      <c r="M24">
+        <v>16</v>
+      </c>
+      <c r="N24">
+        <v>2021</v>
+      </c>
+      <c r="O24">
+        <v>10</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25">
+        <v>-30.9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25">
+        <v>-30.89</v>
+      </c>
+      <c r="G25">
+        <v>116.72</v>
+      </c>
+      <c r="H25">
+        <v>283</v>
+      </c>
+      <c r="I25" t="s">
+        <v>92</v>
+      </c>
+      <c r="J25">
+        <v>94622</v>
+      </c>
+      <c r="K25">
+        <v>1966</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>2021</v>
+      </c>
+      <c r="O25">
+        <v>9</v>
+      </c>
+      <c r="P25">
+        <v>30</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26">
+        <v>33.69</v>
+      </c>
+      <c r="C26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26">
+        <v>33.65</v>
+      </c>
+      <c r="G26">
+        <v>-101.81</v>
+      </c>
+      <c r="H26">
+        <v>993</v>
+      </c>
+      <c r="I26" t="s">
+        <v>82</v>
+      </c>
+      <c r="J26">
+        <v>72267</v>
+      </c>
+      <c r="K26">
+        <v>1947</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>2021</v>
+      </c>
+      <c r="O26">
+        <v>10</v>
+      </c>
+      <c r="P26">
+        <v>2</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27">
+        <v>52.62</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F27">
+        <v>52.49</v>
+      </c>
+      <c r="G27">
+        <v>1.75</v>
+      </c>
+      <c r="H27">
+        <v>25</v>
+      </c>
+      <c r="I27" t="s">
+        <v>113</v>
+      </c>
+      <c r="K27">
+        <v>1889</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>2</v>
+      </c>
+      <c r="N27">
+        <v>2004</v>
+      </c>
+      <c r="O27">
+        <v>12</v>
+      </c>
+      <c r="P27">
+        <v>31</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28">
+        <v>52.62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28">
+        <v>52.49</v>
+      </c>
+      <c r="G28">
+        <v>1.75</v>
+      </c>
+      <c r="H28">
+        <v>25</v>
+      </c>
+      <c r="I28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K28">
+        <v>1889</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>2</v>
+      </c>
+      <c r="N28">
+        <v>2004</v>
+      </c>
+      <c r="O28">
+        <v>12</v>
+      </c>
+      <c r="P28">
+        <v>31</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29">
+        <v>42.81</v>
+      </c>
+      <c r="C29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29">
+        <v>43</v>
+      </c>
+      <c r="G29">
+        <v>-82.3</v>
+      </c>
+      <c r="H29">
+        <v>181</v>
+      </c>
+      <c r="I29" t="s">
+        <v>89</v>
+      </c>
+      <c r="J29">
+        <v>71746</v>
+      </c>
+      <c r="K29">
+        <v>2006</v>
+      </c>
+      <c r="L29">
+        <v>3</v>
+      </c>
+      <c r="M29">
+        <v>20</v>
+      </c>
+      <c r="N29">
+        <v>2021</v>
+      </c>
+      <c r="O29">
+        <v>10</v>
+      </c>
+      <c r="P29">
+        <v>2</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30">
+        <v>42.81</v>
+      </c>
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30">
+        <v>43</v>
+      </c>
+      <c r="G30">
+        <v>-82.3</v>
+      </c>
+      <c r="H30">
+        <v>181</v>
+      </c>
+      <c r="I30" t="s">
+        <v>93</v>
+      </c>
+      <c r="J30">
+        <v>71746</v>
+      </c>
+      <c r="K30">
+        <v>2006</v>
+      </c>
+      <c r="L30">
+        <v>3</v>
+      </c>
+      <c r="M30">
+        <v>20</v>
+      </c>
+      <c r="N30">
+        <v>2021</v>
+      </c>
+      <c r="O30">
+        <v>10</v>
+      </c>
+      <c r="P30">
+        <v>2</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31">
+        <v>-35.270000000000003</v>
+      </c>
+      <c r="C31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" t="s">
+        <v>95</v>
+      </c>
+      <c r="F31">
+        <v>-35.299999999999997</v>
+      </c>
+      <c r="G31">
+        <v>149.19999999999999</v>
+      </c>
+      <c r="H31">
+        <v>578</v>
+      </c>
+      <c r="I31" t="s">
+        <v>96</v>
+      </c>
+      <c r="J31">
+        <v>95926</v>
+      </c>
+      <c r="K31">
+        <v>1939</v>
+      </c>
+      <c r="L31">
+        <v>3</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>2010</v>
+      </c>
+      <c r="O31">
+        <v>12</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32">
+        <v>35.57</v>
+      </c>
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32">
+        <v>35.68</v>
+      </c>
+      <c r="G32">
+        <v>51.32</v>
+      </c>
+      <c r="H32">
+        <v>1191</v>
+      </c>
+      <c r="I32" t="s">
+        <v>116</v>
+      </c>
+      <c r="J32">
+        <v>40754</v>
+      </c>
+      <c r="K32">
+        <v>1944</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>13</v>
+      </c>
+      <c r="N32">
+        <v>2021</v>
+      </c>
+      <c r="O32">
+        <v>10</v>
+      </c>
+      <c r="P32">
+        <v>1</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33">
+        <v>36.07</v>
+      </c>
+      <c r="C33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33">
+        <v>36.049999999999997</v>
+      </c>
+      <c r="G33">
+        <v>114.4</v>
+      </c>
+      <c r="H33">
+        <v>64</v>
+      </c>
+      <c r="I33" t="s">
+        <v>47</v>
+      </c>
+      <c r="J33">
+        <v>53898</v>
+      </c>
+      <c r="K33">
+        <v>1951</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>2021</v>
+      </c>
+      <c r="O33">
+        <v>10</v>
+      </c>
+      <c r="P33">
+        <v>1</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34">
+        <v>42.42</v>
+      </c>
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" t="s">
+        <v>100</v>
+      </c>
+      <c r="F34">
+        <v>42.45</v>
+      </c>
+      <c r="G34">
+        <v>-76.45</v>
+      </c>
+      <c r="H34">
+        <v>293</v>
+      </c>
+      <c r="I34" t="s">
+        <v>101</v>
+      </c>
+      <c r="K34">
+        <v>1893</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>2021</v>
+      </c>
+      <c r="O34">
+        <v>10</v>
+      </c>
+      <c r="P34">
+        <v>1</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="0"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35">
+        <v>38.93</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" t="s">
+        <v>103</v>
+      </c>
+      <c r="F35">
+        <v>38.94</v>
+      </c>
+      <c r="G35">
+        <v>-92.32</v>
+      </c>
+      <c r="H35">
+        <v>235</v>
+      </c>
+      <c r="I35" t="s">
+        <v>104</v>
+      </c>
+      <c r="K35">
+        <v>1997</v>
+      </c>
+      <c r="L35">
+        <v>2</v>
+      </c>
+      <c r="M35">
+        <v>14</v>
+      </c>
+      <c r="N35">
+        <v>2021</v>
+      </c>
+      <c r="O35">
+        <v>10</v>
+      </c>
+      <c r="P35">
+        <v>1</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36">
+        <v>38.93</v>
+      </c>
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" t="s">
+        <v>103</v>
+      </c>
+      <c r="F36">
+        <v>38.94</v>
+      </c>
+      <c r="G36">
+        <v>-92.32</v>
+      </c>
+      <c r="H36">
+        <v>235</v>
+      </c>
+      <c r="I36" t="s">
+        <v>107</v>
+      </c>
+      <c r="K36">
+        <v>1997</v>
+      </c>
+      <c r="L36">
+        <v>2</v>
+      </c>
+      <c r="M36">
+        <v>14</v>
+      </c>
+      <c r="N36">
+        <v>2021</v>
+      </c>
+      <c r="O36">
+        <v>10</v>
+      </c>
+      <c r="P36">
+        <v>1</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37">
+        <v>38.93</v>
+      </c>
+      <c r="C37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" t="s">
+        <v>103</v>
+      </c>
+      <c r="F37">
+        <v>38.94</v>
+      </c>
+      <c r="G37">
+        <v>-92.32</v>
+      </c>
+      <c r="H37">
+        <v>235</v>
+      </c>
+      <c r="I37" t="s">
+        <v>108</v>
+      </c>
+      <c r="K37">
+        <v>1997</v>
+      </c>
+      <c r="L37">
+        <v>2</v>
+      </c>
+      <c r="M37">
+        <v>14</v>
+      </c>
+      <c r="N37">
+        <v>2021</v>
+      </c>
+      <c r="O37">
+        <v>10</v>
+      </c>
+      <c r="P37">
+        <v>1</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fit habitat temperatures without diurnal variation
</commit_message>
<xml_diff>
--- a/Climate station data.xlsx
+++ b/Climate station data.xlsx
@@ -1,13 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11217"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCF8EF7-D692-1B42-AB9F-ABD1DDF1ED97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Climate station data" sheetId="1" r:id="rId4"/>
+    <sheet name="Climate station data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhMDarEkPZknNMn2a6YHRhusIRRYw=="/>
     </ext>
@@ -261,9 +278,6 @@
     <t>USC00083163</t>
   </si>
   <si>
-    <t>Diaphorina citri US Pompano Beach</t>
-  </si>
-  <si>
     <t>POMPANO_BEACH_AIRPARK,_FL</t>
   </si>
   <si>
@@ -367,31 +381,38 @@
   </si>
   <si>
     <t>USC00231803</t>
+  </si>
+  <si>
+    <t>Diaphorina citri US Weston</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -399,41 +420,48 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -623,24 +651,26 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="29.11"/>
-    <col customWidth="1" min="2" max="26" width="10.67"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="2" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,7 +723,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -716,38 +746,38 @@
         <v>2.38</v>
       </c>
       <c r="H2" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="J2" s="1">
-        <v>65344.0</v>
+        <v>65344</v>
       </c>
       <c r="K2" s="1">
-        <v>1941.0</v>
+        <v>1941</v>
       </c>
       <c r="L2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M2" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="N2" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O2" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="P2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q2" s="1">
-        <f t="shared" ref="Q2:Q37" si="1">N2-K2+1</f>
+        <f t="shared" ref="Q2:Q37" si="0">N2-K2+1</f>
         <v>81</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -770,38 +800,38 @@
         <v>2.38</v>
       </c>
       <c r="H3" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="J3" s="1">
-        <v>65344.0</v>
+        <v>65344</v>
       </c>
       <c r="K3" s="1">
-        <v>1941.0</v>
+        <v>1941</v>
       </c>
       <c r="L3" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="N3" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O3" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="P3" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -824,38 +854,38 @@
         <v>3.32</v>
       </c>
       <c r="H4" s="1">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="J4" s="1">
-        <v>65201.0</v>
+        <v>65201</v>
       </c>
       <c r="K4" s="1">
-        <v>1998.0</v>
+        <v>1998</v>
       </c>
       <c r="L4" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="M4" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="N4" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O4" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="P4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -878,38 +908,38 @@
         <v>-1.51</v>
       </c>
       <c r="H5" s="1">
-        <v>316.0</v>
+        <v>316</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J5" s="1">
-        <v>65503.0</v>
+        <v>65503</v>
       </c>
       <c r="K5" s="1">
-        <v>1973.0</v>
+        <v>1973</v>
       </c>
       <c r="L5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O5" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="P5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -932,38 +962,38 @@
         <v>120.28</v>
       </c>
       <c r="H6" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="J6" s="2">
-        <v>58251.0</v>
+        <v>58251</v>
       </c>
       <c r="K6" s="1">
-        <v>1953.0</v>
+        <v>1953</v>
       </c>
       <c r="L6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O6" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="P6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
@@ -986,43 +1016,43 @@
         <v>120.28</v>
       </c>
       <c r="H7" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>34</v>
       </c>
       <c r="J7" s="2">
-        <v>58251.0</v>
+        <v>58251</v>
       </c>
       <c r="K7" s="1">
-        <v>1953.0</v>
+        <v>1953</v>
       </c>
       <c r="L7" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O7" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="P7" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="1">
-        <v>39.88</v>
+        <v>39.880000000000003</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>30</v>
@@ -1040,38 +1070,38 @@
         <v>116.28</v>
       </c>
       <c r="H8" s="1">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>37</v>
       </c>
       <c r="J8" s="1">
-        <v>54511.0</v>
+        <v>54511</v>
       </c>
       <c r="K8" s="1">
-        <v>1951.0</v>
+        <v>1951</v>
       </c>
       <c r="L8" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O8" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="P8" s="1">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="Q8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>71</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
@@ -1088,49 +1118,49 @@
         <v>39</v>
       </c>
       <c r="F9" s="1">
-        <v>36.05</v>
+        <v>36.049999999999997</v>
       </c>
       <c r="G9" s="1">
         <v>114.4</v>
       </c>
       <c r="H9" s="1">
-        <v>64.0</v>
+        <v>64</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>40</v>
       </c>
       <c r="J9" s="1">
-        <v>53898.0</v>
+        <v>53898</v>
       </c>
       <c r="K9" s="1">
-        <v>1951.0</v>
+        <v>1951</v>
       </c>
       <c r="L9" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M9" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="N9" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O9" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="P9" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>71</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="1">
-        <v>38.38</v>
+        <v>38.380000000000003</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -1148,43 +1178,43 @@
         <v>23.75</v>
       </c>
       <c r="H10" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>44</v>
       </c>
       <c r="J10" s="1">
-        <v>16716.0</v>
+        <v>16716</v>
       </c>
       <c r="K10" s="1">
-        <v>1955.0</v>
+        <v>1955</v>
       </c>
       <c r="L10" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="N10" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O10" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="P10" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>67</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="1">
-        <v>38.38</v>
+        <v>38.380000000000003</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>42</v>
@@ -1202,38 +1232,38 @@
         <v>23.75</v>
       </c>
       <c r="H11" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>46</v>
       </c>
       <c r="J11" s="1">
-        <v>16716.0</v>
+        <v>16716</v>
       </c>
       <c r="K11" s="1">
-        <v>1955.0</v>
+        <v>1955</v>
       </c>
       <c r="L11" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M11" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="N11" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O11" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="P11" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>67</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
@@ -1256,38 +1286,38 @@
         <v>-43.35</v>
       </c>
       <c r="H12" s="1">
-        <v>911.0</v>
+        <v>911</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>50</v>
       </c>
       <c r="J12" s="1">
-        <v>83692.0</v>
+        <v>83692</v>
       </c>
       <c r="K12" s="1">
-        <v>1977.0</v>
+        <v>1977</v>
       </c>
       <c r="L12" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="M12" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="N12" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="O12" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="P12" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="Q12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
@@ -1310,38 +1340,38 @@
         <v>-43.35</v>
       </c>
       <c r="H13" s="1">
-        <v>911.0</v>
+        <v>911</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>52</v>
       </c>
       <c r="J13" s="1">
-        <v>83692.0</v>
+        <v>83692</v>
       </c>
       <c r="K13" s="1">
-        <v>1977.0</v>
+        <v>1977</v>
       </c>
       <c r="L13" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="M13" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="N13" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="O13" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="P13" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="Q13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
@@ -1364,43 +1394,43 @@
         <v>-43.35</v>
       </c>
       <c r="H14" s="1">
-        <v>911.0</v>
+        <v>911</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>54</v>
       </c>
       <c r="J14" s="1">
-        <v>83692.0</v>
+        <v>83692</v>
       </c>
       <c r="K14" s="1">
-        <v>1977.0</v>
+        <v>1977</v>
       </c>
       <c r="L14" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="M14" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="N14" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="O14" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="P14" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="Q14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B15" s="1">
-        <v>33.62</v>
+        <v>33.619999999999997</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>56</v>
@@ -1418,38 +1448,38 @@
         <v>133.35</v>
       </c>
       <c r="H15" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>58</v>
       </c>
       <c r="J15" s="1">
-        <v>47893.0</v>
+        <v>47893</v>
       </c>
       <c r="K15" s="1">
-        <v>1951.0</v>
+        <v>1951</v>
       </c>
       <c r="L15" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M15" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="N15" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O15" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="P15" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="Q15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>71</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>59</v>
       </c>
@@ -1472,40 +1502,40 @@
         <v>-90.9</v>
       </c>
       <c r="H16" s="1">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>61</v>
       </c>
       <c r="K16" s="1">
-        <v>1930.0</v>
+        <v>1930</v>
       </c>
       <c r="L16" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M16" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="N16" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="O16" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="P16" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="Q16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B17" s="1">
-        <v>35.38</v>
+        <v>35.380000000000003</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>56</v>
@@ -1523,43 +1553,43 @@
         <v>140.1</v>
       </c>
       <c r="H17" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>64</v>
       </c>
       <c r="J17" s="1">
-        <v>47682.0</v>
+        <v>47682</v>
       </c>
       <c r="K17" s="1">
-        <v>1967.0</v>
+        <v>1967</v>
       </c>
       <c r="L17" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="N17" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O17" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="P17" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B18" s="1">
-        <v>35.38</v>
+        <v>35.380000000000003</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>56</v>
@@ -1577,43 +1607,43 @@
         <v>140.1</v>
       </c>
       <c r="H18" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>66</v>
       </c>
       <c r="J18" s="1">
-        <v>47682.0</v>
+        <v>47682</v>
       </c>
       <c r="K18" s="1">
-        <v>1967.0</v>
+        <v>1967</v>
       </c>
       <c r="L18" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M18" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="N18" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O18" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="P18" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B19" s="1">
-        <v>35.38</v>
+        <v>35.380000000000003</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>56</v>
@@ -1631,38 +1661,38 @@
         <v>140.1</v>
       </c>
       <c r="H19" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>68</v>
       </c>
       <c r="J19" s="1">
-        <v>47682.0</v>
+        <v>47682</v>
       </c>
       <c r="K19" s="1">
-        <v>1967.0</v>
+        <v>1967</v>
       </c>
       <c r="L19" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M19" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="N19" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O19" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="P19" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>69</v>
       </c>
@@ -1685,38 +1715,38 @@
         <v>-1.53</v>
       </c>
       <c r="H20" s="1">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>71</v>
       </c>
       <c r="J20" s="1">
-        <v>3257.0</v>
+        <v>3257</v>
       </c>
       <c r="K20" s="1">
-        <v>1973.0</v>
+        <v>1973</v>
       </c>
       <c r="L20" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M20" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="N20" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O20" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="P20" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
@@ -1739,35 +1769,35 @@
         <v>-80.55</v>
       </c>
       <c r="H21" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>74</v>
       </c>
       <c r="K21" s="1">
-        <v>1990.0</v>
+        <v>1990</v>
       </c>
       <c r="L21" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="M21" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="N21" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O21" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="P21" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="Q21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>75</v>
       </c>
@@ -1787,38 +1817,38 @@
         <v>26.17</v>
       </c>
       <c r="G22" s="1">
-        <v>-81.68</v>
+        <v>-81.680000000000007</v>
       </c>
       <c r="H22" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>77</v>
       </c>
       <c r="K22" s="1">
-        <v>1942.0</v>
+        <v>1942</v>
       </c>
       <c r="L22" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M22" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="N22" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O22" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="P22" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="Q22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>78</v>
       </c>
@@ -1841,37 +1871,37 @@
         <v>-80.2</v>
       </c>
       <c r="H23" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>80</v>
       </c>
       <c r="K23" s="1">
-        <v>1912.0</v>
+        <v>1912</v>
       </c>
       <c r="L23" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="M23" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="N23" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O23" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="P23" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="Q23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>110</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
       <c r="B24" s="1">
         <v>26.24</v>
@@ -1883,7 +1913,7 @@
         <v>48</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F24" s="1">
         <v>26.25</v>
@@ -1892,37 +1922,37 @@
         <v>-80.11</v>
       </c>
       <c r="H24" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="I24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K24" s="1">
+        <v>1998</v>
+      </c>
+      <c r="L24" s="1">
+        <v>3</v>
+      </c>
+      <c r="M24" s="1">
+        <v>16</v>
+      </c>
+      <c r="N24" s="1">
+        <v>2021</v>
+      </c>
+      <c r="O24" s="1">
+        <v>10</v>
+      </c>
+      <c r="P24" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="K24" s="1">
-        <v>1998.0</v>
-      </c>
-      <c r="L24" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="M24" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="N24" s="1">
-        <v>2021.0</v>
-      </c>
-      <c r="O24" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="P24" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="Q24" s="1">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="B25" s="1">
         <v>-30.9</v>
@@ -1934,7 +1964,7 @@
         <v>48</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F25" s="1">
         <v>-30.89</v>
@@ -1943,40 +1973,40 @@
         <v>116.72</v>
       </c>
       <c r="H25" s="1">
-        <v>283.0</v>
+        <v>283</v>
       </c>
       <c r="I25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J25" s="1">
+        <v>94622</v>
+      </c>
+      <c r="K25" s="1">
+        <v>1966</v>
+      </c>
+      <c r="L25" s="1">
+        <v>1</v>
+      </c>
+      <c r="M25" s="1">
+        <v>1</v>
+      </c>
+      <c r="N25" s="1">
+        <v>2021</v>
+      </c>
+      <c r="O25" s="1">
+        <v>9</v>
+      </c>
+      <c r="P25" s="1">
+        <v>30</v>
+      </c>
+      <c r="Q25" s="1">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="J25" s="1">
-        <v>94622.0</v>
-      </c>
-      <c r="K25" s="1">
-        <v>1966.0</v>
-      </c>
-      <c r="L25" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="M25" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="N25" s="1">
-        <v>2021.0</v>
-      </c>
-      <c r="O25" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="P25" s="1">
-        <v>30.0</v>
-      </c>
-      <c r="Q25" s="1">
-        <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="B26" s="1">
         <v>33.69</v>
@@ -1988,7 +2018,7 @@
         <v>48</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F26" s="1">
         <v>33.65</v>
@@ -1997,40 +2027,40 @@
         <v>-101.81</v>
       </c>
       <c r="H26" s="1">
-        <v>993.0</v>
+        <v>993</v>
       </c>
       <c r="I26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J26" s="1">
+        <v>72267</v>
+      </c>
+      <c r="K26" s="1">
+        <v>1947</v>
+      </c>
+      <c r="L26" s="1">
+        <v>1</v>
+      </c>
+      <c r="M26" s="1">
+        <v>1</v>
+      </c>
+      <c r="N26" s="1">
+        <v>2021</v>
+      </c>
+      <c r="O26" s="1">
+        <v>10</v>
+      </c>
+      <c r="P26" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="1">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="J26" s="1">
-        <v>72267.0</v>
-      </c>
-      <c r="K26" s="1">
-        <v>1947.0</v>
-      </c>
-      <c r="L26" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="M26" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="N26" s="1">
-        <v>2021.0</v>
-      </c>
-      <c r="O26" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="P26" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="Q26" s="1">
-        <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="B27" s="1">
         <v>52.62</v>
@@ -2042,7 +2072,7 @@
         <v>48</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F27" s="1">
         <v>52.49</v>
@@ -2051,37 +2081,37 @@
         <v>1.75</v>
       </c>
       <c r="H27" s="1">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="I27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K27" s="1">
+        <v>1889</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1</v>
+      </c>
+      <c r="M27" s="1">
+        <v>2</v>
+      </c>
+      <c r="N27" s="1">
+        <v>2004</v>
+      </c>
+      <c r="O27" s="1">
+        <v>12</v>
+      </c>
+      <c r="P27" s="1">
+        <v>31</v>
+      </c>
+      <c r="Q27" s="1">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="K27" s="1">
-        <v>1889.0</v>
-      </c>
-      <c r="L27" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="M27" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="N27" s="1">
-        <v>2004.0</v>
-      </c>
-      <c r="O27" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="P27" s="1">
-        <v>31.0</v>
-      </c>
-      <c r="Q27" s="1">
-        <f t="shared" si="1"/>
-        <v>116</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="B28" s="1">
         <v>52.62</v>
@@ -2099,37 +2129,37 @@
         <v>1.75</v>
       </c>
       <c r="H28" s="1">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="I28" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K28" s="1">
+        <v>1889</v>
+      </c>
+      <c r="L28" s="1">
+        <v>1</v>
+      </c>
+      <c r="M28" s="1">
+        <v>2</v>
+      </c>
+      <c r="N28" s="1">
+        <v>2004</v>
+      </c>
+      <c r="O28" s="1">
+        <v>12</v>
+      </c>
+      <c r="P28" s="1">
+        <v>31</v>
+      </c>
+      <c r="Q28" s="1">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="K28" s="1">
-        <v>1889.0</v>
-      </c>
-      <c r="L28" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="M28" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="N28" s="1">
-        <v>2004.0</v>
-      </c>
-      <c r="O28" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="P28" s="1">
-        <v>31.0</v>
-      </c>
-      <c r="Q28" s="1">
-        <f t="shared" si="1"/>
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="B29" s="1">
         <v>42.81</v>
@@ -2141,49 +2171,49 @@
         <v>48</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F29" s="1">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="G29" s="1">
         <v>-82.3</v>
       </c>
       <c r="H29" s="1">
-        <v>181.0</v>
+        <v>181</v>
       </c>
       <c r="I29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J29" s="1">
+        <v>71746</v>
+      </c>
+      <c r="K29" s="1">
+        <v>2006</v>
+      </c>
+      <c r="L29" s="1">
+        <v>3</v>
+      </c>
+      <c r="M29" s="1">
+        <v>20</v>
+      </c>
+      <c r="N29" s="1">
+        <v>2021</v>
+      </c>
+      <c r="O29" s="1">
+        <v>10</v>
+      </c>
+      <c r="P29" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q29" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="J29" s="1">
-        <v>71746.0</v>
-      </c>
-      <c r="K29" s="1">
-        <v>2006.0</v>
-      </c>
-      <c r="L29" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="M29" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="N29" s="1">
-        <v>2021.0</v>
-      </c>
-      <c r="O29" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="P29" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="Q29" s="1">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="B30" s="1">
         <v>42.81</v>
@@ -2195,52 +2225,52 @@
         <v>48</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F30" s="1">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="G30" s="1">
         <v>-82.3</v>
       </c>
       <c r="H30" s="1">
-        <v>181.0</v>
+        <v>181</v>
       </c>
       <c r="I30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J30" s="1">
+        <v>71746</v>
+      </c>
+      <c r="K30" s="1">
+        <v>2006</v>
+      </c>
+      <c r="L30" s="1">
+        <v>3</v>
+      </c>
+      <c r="M30" s="1">
+        <v>20</v>
+      </c>
+      <c r="N30" s="1">
+        <v>2021</v>
+      </c>
+      <c r="O30" s="1">
+        <v>10</v>
+      </c>
+      <c r="P30" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q30" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="J30" s="1">
-        <v>71746.0</v>
-      </c>
-      <c r="K30" s="1">
-        <v>2006.0</v>
-      </c>
-      <c r="L30" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="M30" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="N30" s="1">
-        <v>2021.0</v>
-      </c>
-      <c r="O30" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="P30" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="Q30" s="1">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="B31" s="1">
-        <v>-35.27</v>
+        <v>-35.270000000000003</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>56</v>
@@ -2249,49 +2279,49 @@
         <v>48</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F31" s="1">
+        <v>-35.299999999999997</v>
+      </c>
+      <c r="G31" s="1">
+        <v>149.19999999999999</v>
+      </c>
+      <c r="H31" s="1">
+        <v>578</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F31" s="1">
-        <v>-35.3</v>
-      </c>
-      <c r="G31" s="1">
-        <v>149.2</v>
-      </c>
-      <c r="H31" s="1">
-        <v>578.0</v>
-      </c>
-      <c r="I31" s="1" t="s">
+      <c r="J31" s="1">
+        <v>95926</v>
+      </c>
+      <c r="K31" s="1">
+        <v>1939</v>
+      </c>
+      <c r="L31" s="1">
+        <v>3</v>
+      </c>
+      <c r="M31" s="1">
+        <v>1</v>
+      </c>
+      <c r="N31" s="1">
+        <v>2010</v>
+      </c>
+      <c r="O31" s="1">
+        <v>12</v>
+      </c>
+      <c r="P31" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="1">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="J31" s="1">
-        <v>95926.0</v>
-      </c>
-      <c r="K31" s="1">
-        <v>1939.0</v>
-      </c>
-      <c r="L31" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="M31" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="N31" s="1">
-        <v>2010.0</v>
-      </c>
-      <c r="O31" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="P31" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="Q31" s="1">
-        <f t="shared" si="1"/>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="B32" s="1">
         <v>35.57</v>
@@ -2303,7 +2333,7 @@
         <v>48</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F32" s="1">
         <v>35.68</v>
@@ -2312,40 +2342,40 @@
         <v>51.32</v>
       </c>
       <c r="H32" s="1">
-        <v>1191.0</v>
+        <v>1191</v>
       </c>
       <c r="I32" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J32" s="1">
+        <v>40754</v>
+      </c>
+      <c r="K32" s="4">
+        <v>1989</v>
+      </c>
+      <c r="L32" s="1">
+        <v>1</v>
+      </c>
+      <c r="M32" s="4">
+        <v>9</v>
+      </c>
+      <c r="N32" s="1">
+        <v>2021</v>
+      </c>
+      <c r="O32" s="1">
+        <v>10</v>
+      </c>
+      <c r="P32" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="J32" s="1">
-        <v>40754.0</v>
-      </c>
-      <c r="K32" s="4">
-        <v>1989.0</v>
-      </c>
-      <c r="L32" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="M32" s="4">
-        <v>9.0</v>
-      </c>
-      <c r="N32" s="1">
-        <v>2021.0</v>
-      </c>
-      <c r="O32" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="P32" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="Q32" s="1">
-        <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="B33" s="1">
         <v>36.07</v>
@@ -2360,46 +2390,46 @@
         <v>39</v>
       </c>
       <c r="F33" s="1">
-        <v>36.05</v>
+        <v>36.049999999999997</v>
       </c>
       <c r="G33" s="1">
         <v>114.4</v>
       </c>
       <c r="H33" s="1">
-        <v>64.0</v>
+        <v>64</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>40</v>
       </c>
       <c r="J33" s="1">
-        <v>53898.0</v>
+        <v>53898</v>
       </c>
       <c r="K33" s="1">
-        <v>1951.0</v>
+        <v>1951</v>
       </c>
       <c r="L33" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M33" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="N33" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O33" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="P33" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q33" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>71</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B34" s="1">
         <v>42.42</v>
@@ -2411,7 +2441,7 @@
         <v>48</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F34" s="1">
         <v>42.45</v>
@@ -2420,37 +2450,37 @@
         <v>-76.45</v>
       </c>
       <c r="H34" s="1">
-        <v>293.0</v>
+        <v>293</v>
       </c>
       <c r="I34" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K34" s="1">
+        <v>1893</v>
+      </c>
+      <c r="L34" s="1">
+        <v>1</v>
+      </c>
+      <c r="M34" s="1">
+        <v>1</v>
+      </c>
+      <c r="N34" s="1">
+        <v>2021</v>
+      </c>
+      <c r="O34" s="1">
+        <v>10</v>
+      </c>
+      <c r="P34" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="1">
+        <f t="shared" si="0"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="K34" s="1">
-        <v>1893.0</v>
-      </c>
-      <c r="L34" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="M34" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="N34" s="1">
-        <v>2021.0</v>
-      </c>
-      <c r="O34" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="P34" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="Q34" s="1">
-        <f t="shared" si="1"/>
-        <v>129</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="3" t="s">
-        <v>110</v>
       </c>
       <c r="B35" s="1">
         <v>38.93</v>
@@ -2462,7 +2492,7 @@
         <v>48</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F35" s="1">
         <v>38.94</v>
@@ -2471,37 +2501,37 @@
         <v>-92.32</v>
       </c>
       <c r="H35" s="1">
-        <v>235.0</v>
+        <v>235</v>
       </c>
       <c r="I35" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K35" s="1">
+        <v>1997</v>
+      </c>
+      <c r="L35" s="1">
+        <v>2</v>
+      </c>
+      <c r="M35" s="1">
+        <v>14</v>
+      </c>
+      <c r="N35" s="1">
+        <v>2021</v>
+      </c>
+      <c r="O35" s="1">
+        <v>10</v>
+      </c>
+      <c r="P35" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="K35" s="1">
-        <v>1997.0</v>
-      </c>
-      <c r="L35" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="M35" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="N35" s="1">
-        <v>2021.0</v>
-      </c>
-      <c r="O35" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="P35" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="Q35" s="1">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="B36" s="1">
         <v>38.93</v>
@@ -2513,7 +2543,7 @@
         <v>48</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F36" s="1">
         <v>38.94</v>
@@ -2522,37 +2552,37 @@
         <v>-92.32</v>
       </c>
       <c r="H36" s="1">
-        <v>235.0</v>
+        <v>235</v>
       </c>
       <c r="I36" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K36" s="1">
+        <v>1997</v>
+      </c>
+      <c r="L36" s="1">
+        <v>2</v>
+      </c>
+      <c r="M36" s="1">
+        <v>14</v>
+      </c>
+      <c r="N36" s="1">
+        <v>2021</v>
+      </c>
+      <c r="O36" s="1">
+        <v>10</v>
+      </c>
+      <c r="P36" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="K36" s="1">
-        <v>1997.0</v>
-      </c>
-      <c r="L36" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="M36" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="N36" s="1">
-        <v>2021.0</v>
-      </c>
-      <c r="O36" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="P36" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="Q36" s="1">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="B37" s="1">
         <v>38.93</v>
@@ -2564,7 +2594,7 @@
         <v>48</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F37" s="1">
         <v>38.94</v>
@@ -2573,38 +2603,36 @@
         <v>-92.32</v>
       </c>
       <c r="H37" s="1">
-        <v>235.0</v>
+        <v>235</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K37" s="1">
-        <v>1997.0</v>
+        <v>1997</v>
       </c>
       <c r="L37" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M37" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="N37" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="O37" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="P37" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q37" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added better user interfacing for selecting species for which to read the climate data
</commit_message>
<xml_diff>
--- a/Climate station data.xlsx
+++ b/Climate station data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11217"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/c.johnson/Documents/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCF8EF7-D692-1B42-AB9F-ABD1DDF1ED97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66ED7255-1B9E-9647-9940-2C5D658F207A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11080" yWindow="3120" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Climate station data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="142">
   <si>
     <t>Species</t>
   </si>
@@ -384,6 +384,81 @@
   </si>
   <si>
     <t>Diaphorina citri US Weston</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>China Dafeng</t>
+  </si>
+  <si>
+    <t>China Langfang</t>
+  </si>
+  <si>
+    <t>China Xinxiang</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Japan Kochi</t>
+  </si>
+  <si>
+    <t>US Leland</t>
+  </si>
+  <si>
+    <t>Japan Chiba</t>
+  </si>
+  <si>
+    <t>UK Sand Hutton</t>
+  </si>
+  <si>
+    <t>US Homestead</t>
+  </si>
+  <si>
+    <t>US Naples</t>
+  </si>
+  <si>
+    <t>US Weston</t>
+  </si>
+  <si>
+    <t>Australia Yathroo</t>
+  </si>
+  <si>
+    <t>US Lubbock</t>
+  </si>
+  <si>
+    <t>UK Norwich</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Australia Acton</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>China Henan</t>
+  </si>
+  <si>
+    <t>US Ithaca</t>
+  </si>
+  <si>
+    <t>US Columbia</t>
   </si>
 </sst>
 </file>
@@ -658,1975 +733,2087 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="26" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="27" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="1">
         <v>6.45</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>6.35</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>2.38</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>4</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>65344</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>1941</v>
       </c>
-      <c r="L2" s="1">
-        <v>1</v>
-      </c>
       <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
         <v>2</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1">
         <v>2021</v>
       </c>
-      <c r="O2" s="1">
-        <v>10</v>
-      </c>
       <c r="P2" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q2" s="1">
-        <f t="shared" ref="Q2:Q37" si="0">N2-K2+1</f>
+        <v>1</v>
+      </c>
+      <c r="R2" s="1">
+        <f t="shared" ref="R2:R37" si="0">O2-L2+1</f>
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="1">
         <v>6.45</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>6.35</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>2.38</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>4</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>65344</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>1941</v>
       </c>
-      <c r="L3" s="1">
-        <v>1</v>
-      </c>
       <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
         <v>2</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>2021</v>
       </c>
-      <c r="O3" s="1">
-        <v>10</v>
-      </c>
       <c r="P3" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q3" s="1">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1">
         <f t="shared" si="0"/>
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="1">
         <v>7.45</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>6.58</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>3.32</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>41</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>65201</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L4" s="1">
         <v>1998</v>
       </c>
-      <c r="L4" s="1">
-        <v>10</v>
-      </c>
       <c r="M4" s="1">
+        <v>10</v>
+      </c>
+      <c r="N4" s="1">
         <v>5</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O4" s="1">
         <v>2021</v>
       </c>
-      <c r="O4" s="1">
-        <v>10</v>
-      </c>
       <c r="P4" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+      <c r="R4" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="1">
         <v>12.38</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>12.35</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>-1.51</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>316</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>65503</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>1973</v>
       </c>
-      <c r="L5" s="1">
-        <v>1</v>
-      </c>
       <c r="M5" s="1">
         <v>1</v>
       </c>
       <c r="N5" s="1">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
         <v>2021</v>
       </c>
-      <c r="O5" s="1">
-        <v>10</v>
-      </c>
       <c r="P5" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q5" s="1">
+        <v>1</v>
+      </c>
+      <c r="R5" s="1">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="1">
         <v>33.33</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>32.85</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>120.28</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>5</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <v>58251</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <v>1953</v>
       </c>
-      <c r="L6" s="1">
-        <v>1</v>
-      </c>
       <c r="M6" s="1">
         <v>1</v>
       </c>
       <c r="N6" s="1">
+        <v>1</v>
+      </c>
+      <c r="O6" s="1">
         <v>2021</v>
       </c>
-      <c r="O6" s="1">
-        <v>10</v>
-      </c>
       <c r="P6" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q6" s="1">
+        <v>1</v>
+      </c>
+      <c r="R6" s="1">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="1">
         <v>33.33</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>32.85</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>120.28</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>5</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <v>58251</v>
       </c>
-      <c r="K7" s="1">
+      <c r="L7" s="1">
         <v>1953</v>
       </c>
-      <c r="L7" s="1">
-        <v>1</v>
-      </c>
       <c r="M7" s="1">
         <v>1</v>
       </c>
       <c r="N7" s="1">
+        <v>1</v>
+      </c>
+      <c r="O7" s="1">
         <v>2021</v>
       </c>
-      <c r="O7" s="1">
-        <v>10</v>
-      </c>
       <c r="P7" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q7" s="1">
+        <v>1</v>
+      </c>
+      <c r="R7" s="1">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="1">
         <v>39.880000000000003</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>39.93</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>116.28</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>55</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <v>54511</v>
       </c>
-      <c r="K8" s="1">
+      <c r="L8" s="1">
         <v>1951</v>
       </c>
-      <c r="L8" s="1">
-        <v>1</v>
-      </c>
       <c r="M8" s="1">
         <v>1</v>
       </c>
       <c r="N8" s="1">
+        <v>1</v>
+      </c>
+      <c r="O8" s="1">
         <v>2021</v>
       </c>
-      <c r="O8" s="1">
+      <c r="P8" s="1">
         <v>9</v>
       </c>
-      <c r="P8" s="1">
+      <c r="Q8" s="1">
         <v>29</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="R8" s="1">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="1">
         <v>35.53</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>36.049999999999997</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>114.4</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>64</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <v>53898</v>
       </c>
-      <c r="K9" s="1">
+      <c r="L9" s="1">
         <v>1951</v>
       </c>
-      <c r="L9" s="1">
-        <v>1</v>
-      </c>
       <c r="M9" s="1">
         <v>1</v>
       </c>
       <c r="N9" s="1">
+        <v>1</v>
+      </c>
+      <c r="O9" s="1">
         <v>2021</v>
       </c>
-      <c r="O9" s="1">
-        <v>10</v>
-      </c>
       <c r="P9" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q9" s="1">
+        <v>1</v>
+      </c>
+      <c r="R9" s="1">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="1">
         <v>38.380000000000003</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>37.9</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>23.75</v>
       </c>
-      <c r="H10" s="1">
-        <v>10</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="1">
+        <v>10</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <v>16716</v>
       </c>
-      <c r="K10" s="1">
+      <c r="L10" s="1">
         <v>1955</v>
       </c>
-      <c r="L10" s="1">
-        <v>1</v>
-      </c>
       <c r="M10" s="1">
         <v>1</v>
       </c>
       <c r="N10" s="1">
+        <v>1</v>
+      </c>
+      <c r="O10" s="1">
         <v>2021</v>
       </c>
-      <c r="O10" s="1">
-        <v>10</v>
-      </c>
       <c r="P10" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q10" s="1">
+        <v>1</v>
+      </c>
+      <c r="R10" s="1">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="1">
         <v>38.380000000000003</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>37.9</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <v>23.75</v>
       </c>
-      <c r="H11" s="1">
-        <v>10</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="1">
+        <v>10</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <v>16716</v>
       </c>
-      <c r="K11" s="1">
+      <c r="L11" s="1">
         <v>1955</v>
       </c>
-      <c r="L11" s="1">
-        <v>1</v>
-      </c>
       <c r="M11" s="1">
         <v>1</v>
       </c>
       <c r="N11" s="1">
+        <v>1</v>
+      </c>
+      <c r="O11" s="1">
         <v>2021</v>
       </c>
-      <c r="O11" s="1">
-        <v>10</v>
-      </c>
       <c r="P11" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q11" s="1">
+        <v>1</v>
+      </c>
+      <c r="R11" s="1">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="1">
         <v>-21.23</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12" s="1">
         <v>-21.77</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <v>-43.35</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>911</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J12" s="1">
+      <c r="K12" s="1">
         <v>83692</v>
       </c>
-      <c r="K12" s="1">
+      <c r="L12" s="1">
         <v>1977</v>
       </c>
-      <c r="L12" s="1">
-        <v>10</v>
-      </c>
       <c r="M12" s="1">
+        <v>10</v>
+      </c>
+      <c r="N12" s="1">
         <v>24</v>
       </c>
-      <c r="N12" s="1">
+      <c r="O12" s="1">
         <v>2017</v>
       </c>
-      <c r="O12" s="1">
+      <c r="P12" s="1">
         <v>8</v>
       </c>
-      <c r="P12" s="1">
+      <c r="Q12" s="1">
         <v>7</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="R12" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" s="1">
         <v>-21.23</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13" s="1">
         <v>-21.77</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <v>-43.35</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>911</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K13" s="1">
         <v>83692</v>
       </c>
-      <c r="K13" s="1">
+      <c r="L13" s="1">
         <v>1977</v>
       </c>
-      <c r="L13" s="1">
-        <v>10</v>
-      </c>
       <c r="M13" s="1">
+        <v>10</v>
+      </c>
+      <c r="N13" s="1">
         <v>24</v>
       </c>
-      <c r="N13" s="1">
+      <c r="O13" s="1">
         <v>2017</v>
       </c>
-      <c r="O13" s="1">
+      <c r="P13" s="1">
         <v>8</v>
       </c>
-      <c r="P13" s="1">
+      <c r="Q13" s="1">
         <v>7</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="R13" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="1">
         <v>-21.23</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>-21.77</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <v>-43.35</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>911</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J14" s="1">
+      <c r="K14" s="1">
         <v>83692</v>
       </c>
-      <c r="K14" s="1">
+      <c r="L14" s="1">
         <v>1977</v>
       </c>
-      <c r="L14" s="1">
-        <v>10</v>
-      </c>
       <c r="M14" s="1">
+        <v>10</v>
+      </c>
+      <c r="N14" s="1">
         <v>24</v>
       </c>
-      <c r="N14" s="1">
+      <c r="O14" s="1">
         <v>2017</v>
       </c>
-      <c r="O14" s="1">
+      <c r="P14" s="1">
         <v>8</v>
       </c>
-      <c r="P14" s="1">
+      <c r="Q14" s="1">
         <v>7</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="R14" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="1">
         <v>33.619999999999997</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>33.57</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <v>133.35</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>5</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J15" s="1">
+      <c r="K15" s="1">
         <v>47893</v>
       </c>
-      <c r="K15" s="1">
+      <c r="L15" s="1">
         <v>1951</v>
       </c>
-      <c r="L15" s="1">
-        <v>1</v>
-      </c>
       <c r="M15" s="1">
         <v>1</v>
       </c>
       <c r="N15" s="1">
+        <v>1</v>
+      </c>
+      <c r="O15" s="1">
         <v>2021</v>
       </c>
-      <c r="O15" s="1">
+      <c r="P15" s="1">
         <v>9</v>
       </c>
-      <c r="P15" s="1">
+      <c r="Q15" s="1">
         <v>30</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="R15" s="1">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C16" s="1">
         <v>33.42</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <v>33.43</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <v>-90.9</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>39</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K16" s="1">
+      <c r="L16" s="1">
         <v>1930</v>
       </c>
-      <c r="L16" s="1">
+      <c r="M16" s="1">
         <v>2</v>
       </c>
-      <c r="M16" s="1">
-        <v>1</v>
-      </c>
       <c r="N16" s="1">
+        <v>1</v>
+      </c>
+      <c r="O16" s="1">
         <v>2019</v>
       </c>
-      <c r="O16" s="1">
+      <c r="P16" s="1">
         <v>4</v>
       </c>
-      <c r="P16" s="1">
+      <c r="Q16" s="1">
         <v>30</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="R16" s="1">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="1">
         <v>35.380000000000003</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>35.6</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <v>140.1</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>19</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J17" s="1">
+      <c r="K17" s="1">
         <v>47682</v>
       </c>
-      <c r="K17" s="1">
+      <c r="L17" s="1">
         <v>1967</v>
       </c>
-      <c r="L17" s="1">
-        <v>1</v>
-      </c>
       <c r="M17" s="1">
         <v>1</v>
       </c>
       <c r="N17" s="1">
+        <v>1</v>
+      </c>
+      <c r="O17" s="1">
         <v>2021</v>
       </c>
-      <c r="O17" s="1">
-        <v>10</v>
-      </c>
       <c r="P17" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q17" s="1">
+        <v>1</v>
+      </c>
+      <c r="R17" s="1">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" s="1">
         <v>35.380000000000003</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <v>35.6</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <v>140.1</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>19</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J18" s="1">
+      <c r="K18" s="1">
         <v>47682</v>
       </c>
-      <c r="K18" s="1">
+      <c r="L18" s="1">
         <v>1967</v>
       </c>
-      <c r="L18" s="1">
-        <v>1</v>
-      </c>
       <c r="M18" s="1">
         <v>1</v>
       </c>
       <c r="N18" s="1">
+        <v>1</v>
+      </c>
+      <c r="O18" s="1">
         <v>2021</v>
       </c>
-      <c r="O18" s="1">
-        <v>10</v>
-      </c>
       <c r="P18" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q18" s="1">
+        <v>1</v>
+      </c>
+      <c r="R18" s="1">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" s="1">
         <v>35.380000000000003</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>35.6</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <v>140.1</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <v>19</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J19" s="1">
+      <c r="K19" s="1">
         <v>47682</v>
       </c>
-      <c r="K19" s="1">
+      <c r="L19" s="1">
         <v>1967</v>
       </c>
-      <c r="L19" s="1">
-        <v>1</v>
-      </c>
       <c r="M19" s="1">
         <v>1</v>
       </c>
       <c r="N19" s="1">
+        <v>1</v>
+      </c>
+      <c r="O19" s="1">
         <v>2021</v>
       </c>
-      <c r="O19" s="1">
-        <v>10</v>
-      </c>
       <c r="P19" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q19" s="1">
+        <v>1</v>
+      </c>
+      <c r="R19" s="1">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="1">
         <v>54.02</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1">
         <v>54.3</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
         <v>-1.53</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <v>40</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="J20" s="1">
+      <c r="K20" s="1">
         <v>3257</v>
       </c>
-      <c r="K20" s="1">
+      <c r="L20" s="1">
         <v>1973</v>
       </c>
-      <c r="L20" s="1">
-        <v>1</v>
-      </c>
       <c r="M20" s="1">
         <v>1</v>
       </c>
       <c r="N20" s="1">
+        <v>1</v>
+      </c>
+      <c r="O20" s="1">
         <v>2021</v>
       </c>
-      <c r="O20" s="1">
-        <v>10</v>
-      </c>
       <c r="P20" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q20" s="1">
+        <v>1</v>
+      </c>
+      <c r="R20" s="1">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" s="1">
         <v>25.47</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G21" s="1">
         <v>25.5</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
         <v>-80.55</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <v>3</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K21" s="1">
+      <c r="L21" s="1">
         <v>1990</v>
       </c>
-      <c r="L21" s="1">
+      <c r="M21" s="1">
         <v>6</v>
       </c>
-      <c r="M21" s="1">
-        <v>1</v>
-      </c>
       <c r="N21" s="1">
+        <v>1</v>
+      </c>
+      <c r="O21" s="1">
         <v>2021</v>
       </c>
-      <c r="O21" s="1">
-        <v>10</v>
-      </c>
       <c r="P21" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q21" s="1">
         <v>2</v>
       </c>
-      <c r="Q21" s="1">
+      <c r="R21" s="1">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22" s="1">
         <v>26.14</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1">
         <v>26.17</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <v>-81.680000000000007</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I22" s="1">
         <v>12</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K22" s="1">
+      <c r="L22" s="1">
         <v>1942</v>
       </c>
-      <c r="L22" s="1">
+      <c r="M22" s="1">
         <v>3</v>
       </c>
-      <c r="M22" s="1">
-        <v>1</v>
-      </c>
       <c r="N22" s="1">
+        <v>1</v>
+      </c>
+      <c r="O22" s="1">
         <v>2021</v>
       </c>
-      <c r="O22" s="1">
-        <v>10</v>
-      </c>
       <c r="P22" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q22" s="1">
         <v>2</v>
       </c>
-      <c r="Q22" s="1">
+      <c r="R22" s="1">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" s="1">
         <v>26.14</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="1">
         <v>26.1</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
         <v>-80.2</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I23" s="1">
         <v>5</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="K23" s="1">
+      <c r="L23" s="1">
         <v>1912</v>
       </c>
-      <c r="L23" s="1">
+      <c r="M23" s="1">
         <v>11</v>
       </c>
-      <c r="M23" s="1">
-        <v>1</v>
-      </c>
       <c r="N23" s="1">
+        <v>1</v>
+      </c>
+      <c r="O23" s="1">
         <v>2021</v>
       </c>
-      <c r="O23" s="1">
-        <v>10</v>
-      </c>
       <c r="P23" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q23" s="1">
         <v>2</v>
       </c>
-      <c r="Q23" s="1">
+      <c r="R23" s="1">
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" s="1">
         <v>26.24</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G24" s="1">
         <v>26.25</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
         <v>-80.11</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <v>6</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K24" s="1">
+      <c r="L24" s="1">
         <v>1998</v>
       </c>
-      <c r="L24" s="1">
+      <c r="M24" s="1">
         <v>3</v>
       </c>
-      <c r="M24" s="1">
+      <c r="N24" s="1">
         <v>16</v>
       </c>
-      <c r="N24" s="1">
+      <c r="O24" s="1">
         <v>2021</v>
       </c>
-      <c r="O24" s="1">
-        <v>10</v>
-      </c>
       <c r="P24" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q24" s="1">
+        <v>1</v>
+      </c>
+      <c r="R24" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="1">
         <v>-30.9</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>-30.89</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <v>116.72</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <v>283</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J25" s="1">
+      <c r="K25" s="1">
         <v>94622</v>
       </c>
-      <c r="K25" s="1">
+      <c r="L25" s="1">
         <v>1966</v>
       </c>
-      <c r="L25" s="1">
-        <v>1</v>
-      </c>
       <c r="M25" s="1">
         <v>1</v>
       </c>
       <c r="N25" s="1">
+        <v>1</v>
+      </c>
+      <c r="O25" s="1">
         <v>2021</v>
       </c>
-      <c r="O25" s="1">
+      <c r="P25" s="1">
         <v>9</v>
       </c>
-      <c r="P25" s="1">
+      <c r="Q25" s="1">
         <v>30</v>
       </c>
-      <c r="Q25" s="1">
+      <c r="R25" s="1">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="1">
         <v>33.69</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F26" s="1">
+      <c r="G26" s="1">
         <v>33.65</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <v>-101.81</v>
       </c>
-      <c r="H26" s="1">
+      <c r="I26" s="1">
         <v>993</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="J26" s="1">
+      <c r="K26" s="1">
         <v>72267</v>
       </c>
-      <c r="K26" s="1">
+      <c r="L26" s="1">
         <v>1947</v>
       </c>
-      <c r="L26" s="1">
-        <v>1</v>
-      </c>
       <c r="M26" s="1">
         <v>1</v>
       </c>
       <c r="N26" s="1">
+        <v>1</v>
+      </c>
+      <c r="O26" s="1">
         <v>2021</v>
       </c>
-      <c r="O26" s="1">
-        <v>10</v>
-      </c>
       <c r="P26" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q26" s="1">
         <v>2</v>
       </c>
-      <c r="Q26" s="1">
+      <c r="R26" s="1">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="1">
         <v>52.62</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F27" s="1">
+      <c r="G27" s="1">
         <v>52.49</v>
       </c>
-      <c r="G27" s="1">
+      <c r="H27" s="1">
         <v>1.75</v>
       </c>
-      <c r="H27" s="1">
+      <c r="I27" s="1">
         <v>25</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="J27" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K27" s="1">
+      <c r="L27" s="1">
         <v>1889</v>
       </c>
-      <c r="L27" s="1">
-        <v>1</v>
-      </c>
       <c r="M27" s="1">
+        <v>1</v>
+      </c>
+      <c r="N27" s="1">
         <v>2</v>
       </c>
-      <c r="N27" s="1">
+      <c r="O27" s="1">
         <v>2004</v>
       </c>
-      <c r="O27" s="1">
+      <c r="P27" s="1">
         <v>12</v>
       </c>
-      <c r="P27" s="1">
+      <c r="Q27" s="1">
         <v>31</v>
       </c>
-      <c r="Q27" s="1">
+      <c r="R27" s="1">
         <f t="shared" si="0"/>
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C28" s="1">
         <v>52.62</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F28" s="1">
+      <c r="G28" s="1">
         <v>52.49</v>
       </c>
-      <c r="G28" s="1">
+      <c r="H28" s="1">
         <v>1.75</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <v>25</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K28" s="1">
+      <c r="L28" s="1">
         <v>1889</v>
       </c>
-      <c r="L28" s="1">
-        <v>1</v>
-      </c>
       <c r="M28" s="1">
+        <v>1</v>
+      </c>
+      <c r="N28" s="1">
         <v>2</v>
       </c>
-      <c r="N28" s="1">
+      <c r="O28" s="1">
         <v>2004</v>
       </c>
-      <c r="O28" s="1">
+      <c r="P28" s="1">
         <v>12</v>
       </c>
-      <c r="P28" s="1">
+      <c r="Q28" s="1">
         <v>31</v>
       </c>
-      <c r="Q28" s="1">
+      <c r="R28" s="1">
         <f t="shared" si="0"/>
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C29" s="1">
         <v>42.81</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F29" s="1">
+      <c r="G29" s="1">
         <v>43</v>
       </c>
-      <c r="G29" s="1">
+      <c r="H29" s="1">
         <v>-82.3</v>
       </c>
-      <c r="H29" s="1">
+      <c r="I29" s="1">
         <v>181</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J29" s="1">
+      <c r="K29" s="1">
         <v>71746</v>
       </c>
-      <c r="K29" s="1">
+      <c r="L29" s="1">
         <v>2006</v>
       </c>
-      <c r="L29" s="1">
+      <c r="M29" s="1">
         <v>3</v>
       </c>
-      <c r="M29" s="1">
+      <c r="N29" s="1">
         <v>20</v>
       </c>
-      <c r="N29" s="1">
+      <c r="O29" s="1">
         <v>2021</v>
       </c>
-      <c r="O29" s="1">
-        <v>10</v>
-      </c>
       <c r="P29" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q29" s="1">
         <v>2</v>
       </c>
-      <c r="Q29" s="1">
+      <c r="R29" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30" s="1">
         <v>42.81</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F30" s="1">
+      <c r="G30" s="1">
         <v>43</v>
       </c>
-      <c r="G30" s="1">
+      <c r="H30" s="1">
         <v>-82.3</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>181</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="J30" s="1">
+      <c r="K30" s="1">
         <v>71746</v>
       </c>
-      <c r="K30" s="1">
+      <c r="L30" s="1">
         <v>2006</v>
       </c>
-      <c r="L30" s="1">
+      <c r="M30" s="1">
         <v>3</v>
       </c>
-      <c r="M30" s="1">
+      <c r="N30" s="1">
         <v>20</v>
       </c>
-      <c r="N30" s="1">
+      <c r="O30" s="1">
         <v>2021</v>
       </c>
-      <c r="O30" s="1">
-        <v>10</v>
-      </c>
       <c r="P30" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q30" s="1">
         <v>2</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="R30" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C31" s="1">
         <v>-35.270000000000003</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F31" s="1">
+      <c r="G31" s="1">
         <v>-35.299999999999997</v>
       </c>
-      <c r="G31" s="1">
+      <c r="H31" s="1">
         <v>149.19999999999999</v>
       </c>
-      <c r="H31" s="1">
+      <c r="I31" s="1">
         <v>578</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="J31" s="1">
+      <c r="K31" s="1">
         <v>95926</v>
       </c>
-      <c r="K31" s="1">
+      <c r="L31" s="1">
         <v>1939</v>
       </c>
-      <c r="L31" s="1">
+      <c r="M31" s="1">
         <v>3</v>
       </c>
-      <c r="M31" s="1">
-        <v>1</v>
-      </c>
       <c r="N31" s="1">
+        <v>1</v>
+      </c>
+      <c r="O31" s="1">
         <v>2010</v>
       </c>
-      <c r="O31" s="1">
+      <c r="P31" s="1">
         <v>12</v>
       </c>
-      <c r="P31" s="1">
-        <v>1</v>
-      </c>
       <c r="Q31" s="1">
+        <v>1</v>
+      </c>
+      <c r="R31" s="1">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C32" s="1">
         <v>35.57</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F32" s="1">
+      <c r="G32" s="1">
         <v>35.68</v>
       </c>
-      <c r="G32" s="1">
+      <c r="H32" s="1">
         <v>51.32</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <v>1191</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J32" s="1">
+      <c r="K32" s="1">
         <v>40754</v>
       </c>
-      <c r="K32" s="4">
+      <c r="L32" s="4">
         <v>1989</v>
       </c>
-      <c r="L32" s="1">
-        <v>1</v>
-      </c>
-      <c r="M32" s="4">
+      <c r="M32" s="1">
+        <v>1</v>
+      </c>
+      <c r="N32" s="4">
         <v>9</v>
       </c>
-      <c r="N32" s="1">
+      <c r="O32" s="1">
         <v>2021</v>
       </c>
-      <c r="O32" s="1">
-        <v>10</v>
-      </c>
       <c r="P32" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q32" s="1">
+        <v>1</v>
+      </c>
+      <c r="R32" s="1">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33" s="1">
         <v>36.07</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F33" s="1">
+      <c r="G33" s="1">
         <v>36.049999999999997</v>
       </c>
-      <c r="G33" s="1">
+      <c r="H33" s="1">
         <v>114.4</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <v>64</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J33" s="1">
+      <c r="K33" s="1">
         <v>53898</v>
       </c>
-      <c r="K33" s="1">
+      <c r="L33" s="1">
         <v>1951</v>
       </c>
-      <c r="L33" s="1">
-        <v>1</v>
-      </c>
       <c r="M33" s="1">
         <v>1</v>
       </c>
       <c r="N33" s="1">
+        <v>1</v>
+      </c>
+      <c r="O33" s="1">
         <v>2021</v>
       </c>
-      <c r="O33" s="1">
-        <v>10</v>
-      </c>
       <c r="P33" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q33" s="1">
+        <v>1</v>
+      </c>
+      <c r="R33" s="1">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C34" s="1">
         <v>42.42</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F34" s="1">
+      <c r="G34" s="1">
         <v>42.45</v>
       </c>
-      <c r="G34" s="1">
+      <c r="H34" s="1">
         <v>-76.45</v>
       </c>
-      <c r="H34" s="1">
+      <c r="I34" s="1">
         <v>293</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K34" s="1">
+      <c r="L34" s="1">
         <v>1893</v>
       </c>
-      <c r="L34" s="1">
-        <v>1</v>
-      </c>
       <c r="M34" s="1">
         <v>1</v>
       </c>
       <c r="N34" s="1">
+        <v>1</v>
+      </c>
+      <c r="O34" s="1">
         <v>2021</v>
       </c>
-      <c r="O34" s="1">
-        <v>10</v>
-      </c>
       <c r="P34" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q34" s="1">
+        <v>1</v>
+      </c>
+      <c r="R34" s="1">
         <f t="shared" si="0"/>
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C35" s="1">
         <v>38.93</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F35" s="1">
+      <c r="G35" s="1">
         <v>38.94</v>
       </c>
-      <c r="G35" s="1">
+      <c r="H35" s="1">
         <v>-92.32</v>
       </c>
-      <c r="H35" s="1">
+      <c r="I35" s="1">
         <v>235</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K35" s="1">
+      <c r="L35" s="1">
         <v>1997</v>
       </c>
-      <c r="L35" s="1">
+      <c r="M35" s="1">
         <v>2</v>
       </c>
-      <c r="M35" s="1">
+      <c r="N35" s="1">
         <v>14</v>
       </c>
-      <c r="N35" s="1">
+      <c r="O35" s="1">
         <v>2021</v>
       </c>
-      <c r="O35" s="1">
-        <v>10</v>
-      </c>
       <c r="P35" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q35" s="1">
+        <v>1</v>
+      </c>
+      <c r="R35" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36" s="1">
         <v>38.93</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F36" s="1">
+      <c r="G36" s="1">
         <v>38.94</v>
       </c>
-      <c r="G36" s="1">
+      <c r="H36" s="1">
         <v>-92.32</v>
       </c>
-      <c r="H36" s="1">
+      <c r="I36" s="1">
         <v>235</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="K36" s="1">
+      <c r="L36" s="1">
         <v>1997</v>
       </c>
-      <c r="L36" s="1">
+      <c r="M36" s="1">
         <v>2</v>
       </c>
-      <c r="M36" s="1">
+      <c r="N36" s="1">
         <v>14</v>
       </c>
-      <c r="N36" s="1">
+      <c r="O36" s="1">
         <v>2021</v>
       </c>
-      <c r="O36" s="1">
-        <v>10</v>
-      </c>
       <c r="P36" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q36" s="1">
+        <v>1</v>
+      </c>
+      <c r="R36" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37" s="1">
         <v>38.93</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F37" s="1">
+      <c r="G37" s="1">
         <v>38.94</v>
       </c>
-      <c r="G37" s="1">
+      <c r="H37" s="1">
         <v>-92.32</v>
       </c>
-      <c r="H37" s="1">
+      <c r="I37" s="1">
         <v>235</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="J37" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="K37" s="1">
+      <c r="L37" s="1">
         <v>1997</v>
       </c>
-      <c r="L37" s="1">
+      <c r="M37" s="1">
         <v>2</v>
       </c>
-      <c r="M37" s="1">
+      <c r="N37" s="1">
         <v>14</v>
       </c>
-      <c r="N37" s="1">
+      <c r="O37" s="1">
         <v>2021</v>
       </c>
-      <c r="O37" s="1">
-        <v>10</v>
-      </c>
       <c r="P37" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q37" s="1">
+        <v>1</v>
+      </c>
+      <c r="R37" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>

</xml_diff>